<commit_message>
submitted design review 2
</commit_message>
<xml_diff>
--- a/Lab5/circuit/ESP32_Pinout.xlsx
+++ b/Lab5/circuit/ESP32_Pinout.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shalini sarda\Documents\MEAM510\Lab5\circuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{019548D7-70BC-4230-9507-6D168D652B63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB8397E-4D2E-4712-837E-A8975BFD4BBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1230" windowWidth="21600" windowHeight="11505" xr2:uid="{9A9A12BF-547D-4A3C-B900-A4D046723A8E}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{9A9A12BF-547D-4A3C-B900-A4D046723A8E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Motor Circuit" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensor Circuit" sheetId="2" r:id="rId1"/>
+    <sheet name="Sensor Pinouts" sheetId="3" r:id="rId2"/>
+    <sheet name="Motor Circuit" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Motor Circuit'!$B$2:$C$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Motor Circuit'!$B$2:$C$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sensor Circuit'!$B$2:$C$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="88">
   <si>
     <t>D1</t>
   </si>
@@ -222,7 +225,85 @@
     <t>LINK TO OTHER ESP32</t>
   </si>
   <si>
-    <t>ESP32</t>
+    <t>5V Supply</t>
+  </si>
+  <si>
+    <t>Trigger Pulse Input</t>
+  </si>
+  <si>
+    <t>Echo Pulse Output</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>V_Out</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>XSHUT / GPIO0</t>
+  </si>
+  <si>
+    <t>GPIO1</t>
+  </si>
+  <si>
+    <t>VIN (2.8V)</t>
+  </si>
+  <si>
+    <t>ToF Distance Ranging (I2C)</t>
+  </si>
+  <si>
+    <t>Ultrasonic (ADC)</t>
+  </si>
+  <si>
+    <t>Sharp IR (ADC)</t>
+  </si>
+  <si>
+    <t>GPIO 21</t>
+  </si>
+  <si>
+    <t>GPIO 22</t>
+  </si>
+  <si>
+    <t>ToF SCL</t>
+  </si>
+  <si>
+    <t>ToF SDA</t>
+  </si>
+  <si>
+    <t>GPIO 9</t>
+  </si>
+  <si>
+    <t>GPIO 10</t>
+  </si>
+  <si>
+    <t>Ultrasonic Trigger</t>
+  </si>
+  <si>
+    <t>Ultrasonic Echo</t>
+  </si>
+  <si>
+    <t>SHARP IR ADC</t>
+  </si>
+  <si>
+    <t>GPIO 32</t>
+  </si>
+  <si>
+    <t>Master ESP32</t>
+  </si>
+  <si>
+    <t>Secondary ESP32</t>
   </si>
 </sst>
 </file>
@@ -254,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +372,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -304,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -314,6 +401,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,22 +721,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B327C81-8EE4-477F-AEB8-68EE944F1997}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287A1117-6436-4BF9-B45E-5B4576C76D7B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B2:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -678,41 +771,40 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>56</v>
+      <c r="C6" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>56</v>
+      <c r="C7" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="C8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="C10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -726,18 +818,17 @@
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>59</v>
+      <c r="C12" s="8" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="6"/>
+      <c r="C13" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -759,35 +850,35 @@
       <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -795,7 +886,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>26</v>
       </c>
@@ -803,7 +894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>10</v>
       </c>
@@ -811,7 +902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -819,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>28</v>
       </c>
@@ -827,7 +918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>29</v>
       </c>
@@ -835,55 +926,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>38</v>
       </c>
@@ -974,6 +1062,528 @@
   </sheetData>
   <autoFilter ref="B2:C42" xr:uid="{2456D0DB-0239-4557-929E-BC12D4FD1069}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="70" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BC2018-989B-4F22-9DE7-B5DB8AEBC87D}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B327C81-8EE4-477F-AEB8-68EE944F1997}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:D42"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:C42" xr:uid="{2456D0DB-0239-4557-929E-BC12D4FD1069}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="70" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>